<commit_message>
first draft MA done
</commit_message>
<xml_diff>
--- a/models/models.xlsx
+++ b/models/models.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debor\masterThesis\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debor\MA_fork\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C84189-7476-4497-BEC8-DB96F37ACE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFAE8F2-4C1E-4FAF-BAD9-12B5FC420F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{635E8393-0A12-4C55-AB50-6567886706BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{635E8393-0A12-4C55-AB50-6567886706BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>model</t>
   </si>
@@ -54,9 +54,6 @@
     <t>eval_01.txt</t>
   </si>
   <si>
-    <t>CMUSphinx</t>
-  </si>
-  <si>
     <t>eng_latn_uk_broad_filtered, eng_latn_uk_narrow, eng_latn_us_broad_filtered, eng_latn_us_narrow, fre_latn_broad_filtered, fre_latn_narrow, geo_geor_broad_filtered, gre_grek_broad_filtered, gre_grek_narrow, hin_deva_broad_filtered, hin_deva_narrow, jpn_hira_narrow_filtered, kor_hang_narrow_filtered, vie_latn_hanoi_narrow_filtered</t>
   </si>
   <si>
@@ -97,13 +94,40 @@
   </si>
   <si>
     <t>not yet done with training</t>
+  </si>
+  <si>
+    <t>eval_03.txt</t>
+  </si>
+  <si>
+    <t>200,000 steps</t>
+  </si>
+  <si>
+    <t>10,000 steps</t>
+  </si>
+  <si>
+    <t>baseline_short_raw</t>
+  </si>
+  <si>
+    <t>baseline_long_raw</t>
+  </si>
+  <si>
+    <t>baseline_short_clean</t>
+  </si>
+  <si>
+    <t>baseline_long_clean</t>
+  </si>
+  <si>
+    <t>F2_short_clean</t>
+  </si>
+  <si>
+    <t>F2_long_clean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,16 +141,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -134,17 +189,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="20 % - Akzent4" xfId="2" builtinId="42"/>
+    <cellStyle name="20 % - Akzent6" xfId="3" builtinId="50"/>
+    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,16 +551,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8231B97C-203A-4D70-81CA-CB60B4AF272A}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="49" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" style="1" customWidth="1"/>
@@ -476,112 +570,347 @@
     <col min="10" max="11" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="1:13" s="10" customFormat="1" ht="124.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" spans="1:13" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
+        <v>2</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>4</v>
+      </c>
+      <c r="B8" s="8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8">
+        <v>8</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="124.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B12" s="4">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="B13" s="4">
         <v>12</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>